<commit_message>
Update Look and Feel
</commit_message>
<xml_diff>
--- a/CougSat1-Ground/test/TelemetryPacketCalculator.xlsx
+++ b/CougSat1-Ground/test/TelemetryPacketCalculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bradley\Documents\GitHub\CougSat1-Software\CougSat1-Ground\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623717E3-8F0A-4460-ABDC-D96847F70352}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9418F541-460E-4160-8193-73417A2A0EEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{2B14A9BF-534B-4EED-9B86-7C2EE2D06168}"/>
   </bookViews>
@@ -1106,8 +1106,8 @@
   <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E137" sqref="E137"/>
+      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="C19" s="7">
         <f ca="1">NOW()</f>
-        <v>43457.758848379628</v>
+        <v>43458.469142245369</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="F19" t="str">
         <f ca="1">IF(D19&lt;&gt;"",RIGHT(DEC2HEX(IF(D19="Time",(C19-DATE(1970,1,1))*86400,C19/VLOOKUP(D19,Enums!$G$2:$I$20,2,FALSE)),E19*2),E19*2),"")</f>
-        <v>5C1FD01C</v>
+        <v>5C20BFD5</v>
       </c>
       <c r="H19" s="5"/>
     </row>

</xml_diff>